<commit_message>
feat: complete code program
</commit_message>
<xml_diff>
--- a/pharma-ocr/thuoc_detected.xlsx
+++ b/pharma-ocr/thuoc_detected.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R12" sqref="R12"/>
@@ -540,6 +540,141 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>acetylcystein 200 mg f 4</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Thuốc</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>al . £</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Thuốc</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>acetylcystein 200 mg a ze</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Thuốc</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>acetylcystein 200 mg a</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Thuốc</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>‘acehasan 200</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Thuốc</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>acehasan, 200. _</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Thuốc</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>acetylcystein ay)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Thuốc</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>acetylcystein 200 mg a</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Thuốc</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>atp.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Thuốc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>